<commit_message>
RAB-528: Fix invalid trim when file does not start on first column
</commit_message>
<xml_diff>
--- a/components/tailored-import/back/tests/Common/simple_import.xlsx
+++ b/components/tailored-import/back/tests/Common/simple_import.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27720" windowHeight="12570"/>
+    <workbookView windowWidth="27720" windowHeight="14370" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
@@ -63,12 +63,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -82,6 +82,36 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -95,8 +125,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -104,7 +149,60 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -118,104 +216,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -232,6 +232,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -244,175 +250,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -435,15 +435,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -459,17 +450,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -500,26 +500,26 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -528,142 +528,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1013,7 +1013,7 @@
   <sheetPr/>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -1119,8 +1119,8 @@
   <sheetPr/>
   <dimension ref="B2:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6" outlineLevelCol="6"/>
@@ -1170,7 +1170,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="5" customFormat="1" spans="2:7">
+    <row r="5" customFormat="1" spans="2:6">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -1185,10 +1185,6 @@
       </c>
       <c r="F5" s="2">
         <v>44704</v>
-      </c>
-      <c r="G5">
-        <f>D5*1.2</f>
-        <v>16.644</v>
       </c>
     </row>
     <row r="6" customFormat="1" spans="2:7">

</xml_diff>

<commit_message>
RAB-670: Data preview for multiple sources max 1,000 rows (#13592)
* RAB-670: Data preview for multiple sources max 1,000 rows

* Update tests

* Fix lint

* RAB-670: Fix lint

* RAB-670: Fix cannot refresh sample data when all sample data are null

* RAB-670: Fix test

* RAB-670: Fix test

* RAB-670: Fix test

* RAB-670: Fix test

Co-authored-by: Steven VAIDIE <steven.vaidie@gmail.com>
</commit_message>
<xml_diff>
--- a/components/tailored-import/back/tests/Common/simple_import.xlsx
+++ b/components/tailored-import/back/tests/Common/simple_import.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27720" windowHeight="14370" activeTab="1"/>
+    <workbookView windowWidth="27720" windowHeight="12690" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
     <sheet name="Empty lines and columns" sheetId="2" r:id="rId2"/>
     <sheet name="Empty sheet" sheetId="3" r:id="rId3"/>
     <sheet name="Out of bound value" sheetId="4" r:id="rId4"/>
+    <sheet name="Two lines" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="13">
   <si>
     <t>Sku</t>
   </si>
@@ -62,13 +63,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="m/d/yyyy;@"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  <numFmts count="7">
+    <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="177" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="mmm\-yy"/>
+    <numFmt numFmtId="181" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="182" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -79,11 +81,49 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -111,22 +151,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -134,90 +174,52 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -232,6 +234,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -244,19 +264,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -268,19 +378,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,127 +408,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -423,80 +425,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -519,7 +447,81 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -528,148 +530,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -677,19 +679,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1014,7 +1016,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F3" sqref="A1:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="14.25" outlineLevelRow="5" outlineLevelCol="5"/>
@@ -1119,7 +1121,7 @@
   <sheetPr/>
   <dimension ref="B2:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -1337,4 +1339,84 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="3" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1">
+        <v>12</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>44642</v>
+      </c>
+      <c r="F2">
+        <f>C2*1.2</f>
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1">
+        <v>13.87</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>44704</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5">
+      <c r="C4" s="1"/>
+      <c r="D4"/>
+      <c r="E4" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
RAB-599: Fix invalid file
</commit_message>
<xml_diff>
--- a/components/tailored-import/back/tests/Common/simple_import.xlsx
+++ b/components/tailored-import/back/tests/Common/simple_import.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Empty sheet" sheetId="3" r:id="rId3"/>
     <sheet name="Out of bound value" sheetId="4" r:id="rId4"/>
     <sheet name="Empty header" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="8" r:id="rId6"/>
+    <sheet name="Two lines" sheetId="8" r:id="rId6"/>
     <sheet name="Trailing empty header" sheetId="6" r:id="rId7"/>
     <sheet name="More than 500 cols" sheetId="7" r:id="rId8"/>
   </sheets>
@@ -2967,7 +2967,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="14.25" outlineLevelRow="5" outlineLevelCol="5"/>

</xml_diff>